<commit_message>
Fixed bugs and Updated sprint
- Fixed bug where moving task to stage with assigned group doesn't remove assigned employee, if employee isn't in said group

- Moving tasks now displays a warning about moving to stage with assigned groups can remove current assignee, if said assignee isn't part of assigned group

-Updated sprint backlog
</commit_message>
<xml_diff>
--- a/Sprints/Sprint4/G4CapstoneProject_Sprint4_Backlog_Burndown.xlsx
+++ b/Sprints/Sprint4/G4CapstoneProject_Sprint4_Backlog_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Documents\GitHub\Capstone-Project\Sprints\Sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38128F41-8CBA-423B-B227-88C37C2CBDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A64DFA4-8E83-4972-BF74-D2A0F783A9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5265" yWindow="3990" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Related User Story</t>
   </si>
@@ -329,6 +329,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -351,9 +354,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -471,10 +471,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>18.55</c:v>
+                  <c:v>15.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1522,7 +1522,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,105 +1536,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="6">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="8">
-        <v>2</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="13"/>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="13"/>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -1650,7 +1666,7 @@
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -1666,7 +1682,7 @@
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="10" t="s">
         <v>31</v>
       </c>
@@ -1680,7 +1696,7 @@
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1700,7 +1716,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="11" t="s">
         <v>19</v>
       </c>
@@ -1718,7 +1734,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="14" t="s">
         <v>20</v>
       </c>
@@ -1736,7 +1752,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="14" t="s">
         <v>21</v>
       </c>
@@ -1754,7 +1770,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -1774,7 +1790,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
@@ -1792,7 +1808,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1826,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
@@ -1834,11 +1850,11 @@
       </c>
       <c r="C19" s="4">
         <f>SUM(C4:C18)</f>
-        <v>18.55</v>
+        <v>15.55</v>
       </c>
       <c r="D19" s="4">
         <f>SUM(D4:D18)</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E19" s="4">
         <f>SUM(E4:E18)</f>

</xml_diff>